<commit_message>
Updates of the code and debugging
</commit_message>
<xml_diff>
--- a/backend/tasks.xlsx
+++ b/backend/tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Zahra\PhD topic\Python\React\TaskMind\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879565B4-DDC0-4D06-8E1C-9D3831C05EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91F7085-EDF9-448E-8F75-9327541E0540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="74">
   <si>
     <t>TaskID</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Inspection1.jpg</t>
   </si>
   <si>
-    <t>Inspection 7</t>
-  </si>
-  <si>
     <t>RobotCode</t>
   </si>
   <si>
@@ -195,63 +192,6 @@
     <t>Inspection</t>
   </si>
   <si>
-    <t xml:space="preserve">Take the base hospital part and place it in the right direction, so the wholes match the nuts in the buttom. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the hospital part which has a round roof and place it on top of hospital base. </t>
-  </si>
-  <si>
-    <t>Take the hospital part which has a "H" sign and place it on top of hospital base to fit.</t>
-  </si>
-  <si>
-    <t>Take two screws and fix the top parts of the hospital to their place. You can use the screwdriver if you need.</t>
-  </si>
-  <si>
-    <t>Take the bridge building with sharp roof and place it in the inner hole. Pay attention to the direction of the building.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the bridge building with flat roof and place it in the otter hole. Pay attention to the direction of the building. </t>
-  </si>
-  <si>
-    <t>Guide the bridge rod through the wholes of both buildings.</t>
-  </si>
-  <si>
-    <t>Take the dovetail building and place it in the same direction as shown in the photo.</t>
-  </si>
-  <si>
-    <t>Take the top part of dovetail and snip it over the buttom dovetail.</t>
-  </si>
-  <si>
-    <t>Take the wheel holder and place it in location.</t>
-  </si>
-  <si>
-    <t>Take two screws and fix the Wheel holder part in place.</t>
-  </si>
-  <si>
-    <t>Take the wheel and place it in the middle of wheel holder.</t>
-  </si>
-  <si>
-    <t>Take a screw and a nut and fix the sheel in place.</t>
-  </si>
-  <si>
-    <t>Take the triangle building and place it.</t>
-  </si>
-  <si>
-    <t>Take the buttom Snap building, the biggest part, and place it in the direction as shown in the photo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take the Middle snap building and place it on top of the buttom snap. </t>
-  </si>
-  <si>
-    <t>Take the top part of Snap building and place it on top of the middle part.</t>
-  </si>
-  <si>
-    <t>Take the museum building and place it.</t>
-  </si>
-  <si>
-    <t>Please wait till the robot finish it's tasks. Inspect the final assembly, check if everything is correctly placed. If yes click on Finish button.</t>
-  </si>
-  <si>
     <t>Hospital_big_top</t>
   </si>
   <si>
@@ -259,6 +199,66 @@
   </si>
   <si>
     <t>Hospital_small_top, Hospital_big_top</t>
+  </si>
+  <si>
+    <t>ImageNameRobot</t>
+  </si>
+  <si>
+    <t>Place the hospital base so its holes match the nuts at the bottom.</t>
+  </si>
+  <si>
+    <t>Place the round-roof hospital part on top of the base.</t>
+  </si>
+  <si>
+    <t>Place the “H” sign hospital part on top of the base to fit.</t>
+  </si>
+  <si>
+    <t>Fix the top parts of the hospital with two screws.</t>
+  </si>
+  <si>
+    <t>Place the sharp-roof bridge in the inner hole, facing the right direction.</t>
+  </si>
+  <si>
+    <t>Place the flat-roof bridge in the outer hole, facing the right direction.</t>
+  </si>
+  <si>
+    <t>Insert the bridge rod through both buildings.</t>
+  </si>
+  <si>
+    <t>Place the dovetail building in the shown direction.</t>
+  </si>
+  <si>
+    <t>Snap the top dovetail part over the bottom.</t>
+  </si>
+  <si>
+    <t>Place the wheel holder in position.</t>
+  </si>
+  <si>
+    <t>Fix the wheel holder with two screws.</t>
+  </si>
+  <si>
+    <t>Place the wheel in the wheel holder.</t>
+  </si>
+  <si>
+    <t>Place the triangle building.</t>
+  </si>
+  <si>
+    <t>Place the largest Snap building as shown.</t>
+  </si>
+  <si>
+    <t>Place the middle Snap building on top of the bottom.</t>
+  </si>
+  <si>
+    <t>Place the top Snap building on the middle part.</t>
+  </si>
+  <si>
+    <t>Place the museum building.</t>
+  </si>
+  <si>
+    <t>Wait for the robot to finish, inspect the assembly, and click Finish if correct.</t>
+  </si>
+  <si>
+    <t>Align the holes and fix the wheel with a screw and nut. Pay attention, you need longer screws for this task.</t>
   </si>
 </sst>
 </file>
@@ -602,24 +602,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="53.5546875" customWidth="1"/>
-    <col min="4" max="4" width="28.21875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="28.109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="4" max="5" width="28.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -633,22 +633,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -656,86 +659,95 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4">
         <v>21</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="2"/>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>1+A2</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4">
         <v>12</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>30</v>
       </c>
-      <c r="G3" t="s">
-        <v>71</v>
-      </c>
       <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A20" si="0">1+A3</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="4">
         <v>35</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>30</v>
       </c>
-      <c r="G4" t="s">
-        <v>72</v>
-      </c>
       <c r="H4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -744,82 +756,91 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4">
         <v>21</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1">
         <v>20</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>30</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="I6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="4">
         <v>10</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>30</v>
       </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -828,28 +849,31 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4">
         <v>6</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>100</v>
       </c>
-      <c r="G8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -858,55 +882,61 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4">
         <v>7</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>35</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>12</v>
       </c>
-      <c r="I9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4">
         <v>12</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>25</v>
       </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
       <c r="H10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" t="s">
         <v>12</v>
       </c>
-      <c r="I10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -915,25 +945,28 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="4">
         <v>20</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>32</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>15</v>
       </c>
-      <c r="I11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -942,58 +975,64 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="4">
         <v>45</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>40</v>
       </c>
-      <c r="G12" t="s">
-        <v>40</v>
-      </c>
       <c r="H12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" t="s">
         <v>15</v>
       </c>
-      <c r="I12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="4">
         <v>35</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="4">
         <v>30</v>
       </c>
-      <c r="G13" t="s">
-        <v>37</v>
-      </c>
       <c r="H13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" t="s">
         <v>17</v>
       </c>
-      <c r="I13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1002,28 +1041,31 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="4">
+        <v>20</v>
+      </c>
+      <c r="G14" s="4">
         <v>100</v>
       </c>
-      <c r="G14" t="s">
-        <v>40</v>
-      </c>
       <c r="H14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="J14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1032,25 +1074,28 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="4">
         <v>32</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>40</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>21</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1059,55 +1104,61 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="4">
         <v>60</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>30</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>29</v>
       </c>
-      <c r="I16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="4">
+        <v>42</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="4">
         <v>20</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G17" s="4">
         <v>100</v>
       </c>
-      <c r="G17" t="s">
-        <v>40</v>
-      </c>
       <c r="H17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" t="s">
         <v>29</v>
       </c>
-      <c r="I17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1116,28 +1167,31 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="4">
         <v>60</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G18" s="4">
         <v>100</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" t="s">
         <v>40</v>
       </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1146,52 +1200,58 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="4">
         <v>52</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>32</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>6</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="4">
         <v>15</v>
       </c>
-      <c r="F20" s="4">
+      <c r="G20" s="4">
         <v>100</v>
       </c>
-      <c r="G20" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
     </row>
   </sheetData>
@@ -1201,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E446E5-85DE-4FD9-98F7-92D9EA47C386}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,7 +1277,7 @@
     <col min="8" max="8" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1231,22 +1291,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1254,86 +1317,95 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4">
         <v>21</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I2" s="2"/>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>1+A2</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4">
         <v>12</v>
       </c>
-      <c r="F3" s="4">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>71</v>
+      <c r="G3" s="4">
+        <v>30</v>
       </c>
       <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A5" si="0">1+A3</f>
+        <f t="shared" ref="A4:A6" si="0">1+A3</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="4">
         <v>35</v>
       </c>
-      <c r="F4" s="4">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s">
-        <v>72</v>
+      <c r="G4" s="4">
+        <v>30</v>
       </c>
       <c r="H4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1342,25 +1414,58 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4">
         <v>21</v>
       </c>
-      <c r="F5" s="4">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
+      <c r="G5" s="4">
+        <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4">
+        <v>15</v>
+      </c>
+      <c r="G6" s="4">
+        <v>100</v>
+      </c>
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>